<commit_message>
Fix testing names, added an additional test
</commit_message>
<xml_diff>
--- a/TestSuite.xlsx
+++ b/TestSuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>S. No.</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Boundary</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Min -</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Int32.MaxValue</t>
   </si>
 </sst>
 </file>
@@ -451,12 +463,13 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -621,23 +634,59 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>-50</v>
+      </c>
+      <c r="C10">
+        <v>-50</v>
+      </c>
+      <c r="D10">
+        <v>-50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>